<commit_message>
Added files for Shades
</commit_message>
<xml_diff>
--- a/shades/hardware_design/Shades.xlsx
+++ b/shades/hardware_design/Shades.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="10400" yWindow="5140" windowWidth="35540" windowHeight="20080" tabRatio="311"/>
   </bookViews>
   <sheets>
-    <sheet name="Shades v3.1" sheetId="1" r:id="rId1"/>
+    <sheet name="Shades v4.0" sheetId="2" r:id="rId1"/>
+    <sheet name="Shades v3.1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="160">
   <si>
     <t>Index</t>
   </si>
@@ -304,6 +305,201 @@
   </si>
   <si>
     <t>29.2 x 106.7 ; 2 layers</t>
+  </si>
+  <si>
+    <t>Shades, v4.0</t>
+  </si>
+  <si>
+    <t>Mouser P/N</t>
+  </si>
+  <si>
+    <t>R1, R2, R5, R6, R7, R8, R11, R12, R13, R14, R15, R16, R17, R18, R19, R22, R23, R24, R25, R27, R29</t>
+  </si>
+  <si>
+    <t>Resistor, thin film</t>
+  </si>
+  <si>
+    <t>667-ERA-2AEB104X</t>
+  </si>
+  <si>
+    <t>Panasonic ERA-2AEB104X</t>
+  </si>
+  <si>
+    <t>R4, R10, R21</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>&lt;= 1%, &gt;= 200mW</t>
+  </si>
+  <si>
+    <t>667-ERJ-PA3D1001V</t>
+  </si>
+  <si>
+    <t>Panasonic ERJ-PA3D1001V</t>
+  </si>
+  <si>
+    <t>R26, R30, R31</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>3.3k</t>
+  </si>
+  <si>
+    <t>C1, C5</t>
+  </si>
+  <si>
+    <t>&gt;= 35V, X?R, &lt;= 20%</t>
+  </si>
+  <si>
+    <t>963-GMK325AB7106MM-T</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden GMK325AB7106MM-T</t>
+  </si>
+  <si>
+    <t>C2, C3, C6, C7, C9, C10, C11, C12, C14, C15, C16</t>
+  </si>
+  <si>
+    <t>&gt;= 25V, X5R, &lt;= 20%</t>
+  </si>
+  <si>
+    <t>710-885012105018</t>
+  </si>
+  <si>
+    <t>Würth 885012105018</t>
+  </si>
+  <si>
+    <t>C4, C8, C13</t>
+  </si>
+  <si>
+    <t>&gt;= 50V, C0G, &lt;= 5%</t>
+  </si>
+  <si>
+    <t>81-GCM1555C1H220JA6D</t>
+  </si>
+  <si>
+    <t>Murata GCM1555C1H220JA16D</t>
+  </si>
+  <si>
+    <t>D3, D4, D5, D6, D7, D8</t>
+  </si>
+  <si>
+    <t>Ceradiode</t>
+  </si>
+  <si>
+    <t>Epcos / TDK B72500D160H60</t>
+  </si>
+  <si>
+    <t>OPA1678 dual op-amp</t>
+  </si>
+  <si>
+    <t>VSSOP8</t>
+  </si>
+  <si>
+    <t>595-OPA1678IDGKT</t>
+  </si>
+  <si>
+    <t>Texas Instruments OPA1678IDGKT</t>
+  </si>
+  <si>
+    <t>B grade (0.2%, 100ppm)</t>
+  </si>
+  <si>
+    <t>595-LM4040B10IDBZR</t>
+  </si>
+  <si>
+    <t>Texas Instruments LM4040B10IDBZ</t>
+  </si>
+  <si>
+    <t>LM324 quad op-amp</t>
+  </si>
+  <si>
+    <t>TSSOP14</t>
+  </si>
+  <si>
+    <t>595-LM324PWR</t>
+  </si>
+  <si>
+    <t>Texas instruments LM324PWR</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>EMI Filter Bead</t>
+  </si>
+  <si>
+    <t>&gt;= 1k ohm, 300mA</t>
+  </si>
+  <si>
+    <t>710-742792664</t>
+  </si>
+  <si>
+    <t>Würth Electronics 742792664</t>
+  </si>
+  <si>
+    <t>LED1, LED3, LED5</t>
+  </si>
+  <si>
+    <t>LED 3mm, mint green</t>
+  </si>
+  <si>
+    <t>Optosupply OSC54L3131A</t>
+  </si>
+  <si>
+    <t>LED2, LED4, LED6</t>
+  </si>
+  <si>
+    <t>LED 3mm, baby pink</t>
+  </si>
+  <si>
+    <t>Optosupply OSC84L3131A</t>
+  </si>
+  <si>
+    <t>Led holder</t>
+  </si>
+  <si>
+    <t>749-ELM-4-350</t>
+  </si>
+  <si>
+    <t>Bivar ELM 2-340</t>
+  </si>
+  <si>
+    <t>R3, R9, R20</t>
+  </si>
+  <si>
+    <t>Slide switch, DPDT</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>2x5 male boxed header, 2.54mm pitch</t>
+  </si>
+  <si>
+    <t>710-61201021621</t>
+  </si>
+  <si>
+    <t>JP1, JP2, JP3</t>
+  </si>
+  <si>
+    <t>855-M7582-46</t>
+  </si>
+  <si>
+    <t>29.2 x 106.7, 4 layers</t>
+  </si>
+  <si>
+    <t>871-B72500D160H60</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/thonkiconn/</t>
   </si>
 </sst>
 </file>
@@ -313,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000000000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -384,6 +580,16 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -461,7 +667,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -558,6 +764,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -567,7 +776,80 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -977,10 +1259,618 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="21" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" customHeight="1">
+      <c r="A1" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" ht="12" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="33">
+      <c r="A4" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="39">
+        <v>21</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="40" t="str">
+        <f>"&lt;= 0.1%, 62.5mW"</f>
+        <v>&lt;= 0.1%, 62.5mW</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="41" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="39">
+        <v>3</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="41" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="39">
+        <v>3</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="40" t="str">
+        <f>"&lt;= 1%, 62.5mW"</f>
+        <v>&lt;= 1%, 62.5mW</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="41" t="str">
+        <f t="shared" ref="F6:F7" si="0">"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="39">
+        <v>1</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="40" t="str">
+        <f>"&lt;= 1%, 62.5mW"</f>
+        <v>&lt;= 1%, 62.5mW</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>0402</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="43"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="40">
+        <v>2</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="41" t="str">
+        <f>"1210"</f>
+        <v>1210</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="22">
+      <c r="A9" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="40">
+        <v>11</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="41" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="40">
+        <v>3</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="46" t="str">
+        <f>"0402"</f>
+        <v>0402</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="48">
+        <v>2</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="40">
+        <v>6</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="50">
+        <v>4</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="40">
+        <v>1</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12" customHeight="1">
+      <c r="A15" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="48">
+        <v>1</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="40">
+        <v>2</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="51" t="str">
+        <f>"0603"</f>
+        <v>0603</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="40">
+        <v>6</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="H18" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="40">
+        <v>3</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="H19" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="40">
+        <v>3</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="H20" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="54" t="str">
+        <f>"- LED1, LED2, LED3, LED4, LED5, LED6"</f>
+        <v>- LED1, LED2, LED3, LED4, LED5, LED6</v>
+      </c>
+      <c r="B21" s="40">
+        <v>6</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="40">
+        <v>3</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="H22" s="60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="40">
+        <v>3</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="42">
+        <v>1</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="48"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="8">
+        <v>3</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="38" t="str">
+        <f>"- JP1, JP2, JP3"</f>
+        <v>- JP1, JP2, JP3</v>
+      </c>
+      <c r="B27" s="23">
+        <v>3</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A17:G17"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -997,16 +1887,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="12" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1035,15 +1925,15 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="12" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
@@ -1310,15 +2200,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="12" customHeight="1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8">
@@ -1493,7 +2383,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="14"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="35"/>
+      <c r="I25" s="61"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="27" t="s">

</xml_diff>